<commit_message>
Se finaliza agregar y editar con jquery
</commit_message>
<xml_diff>
--- a/other/DATA_SISGESTION_Nestor.xlsx
+++ b/other/DATA_SISGESTION_Nestor.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SistemaGestionNestorRey\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B78A299-4FF8-4BB5-9602-81AD61AFBE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20F987E-B860-4606-A279-852E5D149B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{64D24DBD-44EE-466C-ADE8-9B0DE2C0EE37}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
-    <sheet name="AUTOS" sheetId="3" r:id="rId2"/>
-    <sheet name="CLIENTES" sheetId="4" r:id="rId3"/>
-    <sheet name="MARCAS Y MODELOS" sheetId="5" r:id="rId4"/>
+    <sheet name="DISEÑO PAGINA" sheetId="6" r:id="rId2"/>
+    <sheet name="AUTOS" sheetId="3" r:id="rId3"/>
+    <sheet name="CLIENTES" sheetId="4" r:id="rId4"/>
+    <sheet name="MARCAS Y MODELOS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="77">
   <si>
     <t>AUTOS</t>
   </si>
@@ -248,13 +248,34 @@
   </si>
   <si>
     <t>Guardar</t>
+  </si>
+  <si>
+    <t>ESTADOS</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>Entregado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Cancelado</t>
+  </si>
+  <si>
+    <t>LISTADO CLIENTES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +310,14 @@
       <color rgb="FF8900B4"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -606,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -699,6 +728,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -708,6 +758,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -717,9 +806,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -745,45 +831,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,6 +857,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -819,30 +878,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1658,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039C5167-16CD-44EC-8879-3C40CCDAB863}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1712,7 @@
     <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1689,8 +1728,14 @@
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1706,8 +1751,11 @@
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1723,8 +1771,11 @@
       <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1740,8 +1791,11 @@
       <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1751,8 +1805,11 @@
       <c r="E5" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1760,51 +1817,210 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9980C8-7DE9-4675-A99D-20A2352C65BC}">
+  <dimension ref="C2:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
+    </row>
+    <row r="4" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="58"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="60"/>
+    </row>
+    <row r="5" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="32"/>
+      <c r="D5" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34"/>
+    </row>
+    <row r="7" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="43"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+    </row>
+    <row r="8" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="68"/>
+      <c r="E9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="70"/>
+      <c r="H9" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="51"/>
+      <c r="E10" s="33">
+        <v>1165006784</v>
+      </c>
+      <c r="F10" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="71"/>
+      <c r="H10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="85"/>
+    </row>
+    <row r="11" spans="3:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="61"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="63"/>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="61"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
+    </row>
+    <row r="15" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="C11:H15"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E5F623-2172-4AFE-A1E7-9EB4937D4367}">
   <dimension ref="C3:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -1815,44 +2031,44 @@
   <sheetData>
     <row r="3" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="60"/>
     </row>
     <row r="6" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="58"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="3"/>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="59"/>
-      <c r="P6" s="35" t="s">
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="53"/>
+      <c r="P6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="37"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="57"/>
     </row>
     <row r="7" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
@@ -1882,10 +2098,10 @@
       <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="49"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -2003,14 +2219,14 @@
       </c>
     </row>
     <row r="12" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="63"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -2021,17 +2237,17 @@
       <c r="S12" s="3"/>
     </row>
     <row r="13" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="56" t="s">
+      <c r="K13" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="58"/>
+      <c r="L13" s="52"/>
       <c r="M13" s="3"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="4"/>
@@ -2039,28 +2255,28 @@
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
       <c r="M14" s="3"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="23" t="s">
@@ -2079,21 +2295,21 @@
       </c>
     </row>
     <row r="16" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="66"/>
     </row>
     <row r="19" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="9" t="s">
@@ -2104,12 +2320,12 @@
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="29"/>
-      <c r="J21" s="32" t="s">
+      <c r="J21" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="34"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
     </row>
     <row r="22" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="27"/>
@@ -2119,10 +2335,10 @@
       <c r="J22" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="48" t="s">
+      <c r="K22" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="49"/>
+      <c r="L22" s="43"/>
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="4:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2132,10 +2348,10 @@
       <c r="E23" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="80" t="s">
+      <c r="F23" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="81"/>
+      <c r="G23" s="38"/>
       <c r="J23" s="13"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -2166,10 +2382,10 @@
       <c r="E25" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="80" t="s">
+      <c r="F25" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="81"/>
+      <c r="G25" s="38"/>
       <c r="J25" s="18" t="s">
         <v>35</v>
       </c>
@@ -2188,12 +2404,12 @@
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="29"/>
-      <c r="J26" s="50" t="s">
+      <c r="J26" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="52"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="46"/>
     </row>
     <row r="27" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="7" t="s">
@@ -2204,16 +2420,16 @@
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="29"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="52"/>
-      <c r="P27" s="32" t="s">
+      <c r="J27" s="44"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="46"/>
+      <c r="P27" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="34"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="41"/>
       <c r="U27" s="1" t="s">
         <v>45</v>
       </c>
@@ -2223,10 +2439,10 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="29"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="52"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="46"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
@@ -2240,10 +2456,10 @@
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="29"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="55"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="49"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
@@ -2259,16 +2475,16 @@
       <c r="E30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="80" t="s">
+      <c r="F30" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="81"/>
+      <c r="G30" s="38"/>
       <c r="J30" s="5"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="78" t="s">
+      <c r="L30" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="M30" s="79"/>
+      <c r="M30" s="36"/>
       <c r="P30" s="2" t="s">
         <v>15</v>
       </c>
@@ -2383,6 +2599,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="P27:S27"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C12:H16"/>
     <mergeCell ref="L30:M30"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="F25:G25"/>
@@ -2397,11 +2618,6 @@
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="D20:G20"/>
-    <mergeCell ref="P27:S27"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C12:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2409,12 +2625,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D84D248-9681-418F-9233-9DF87A5E27A6}">
   <dimension ref="C3:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="C4" sqref="C4:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,38 +2640,38 @@
   <sheetData>
     <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="60"/>
     </row>
     <row r="6" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="58"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="3"/>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="41"/>
     </row>
     <row r="7" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
@@ -2467,20 +2683,20 @@
       <c r="J7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="66" t="s">
+      <c r="K7" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="67"/>
-      <c r="M7" s="68"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="74"/>
     </row>
     <row r="8" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="49"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -2499,24 +2715,24 @@
       <c r="J9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="39">
+      <c r="K9" s="58">
         <v>1165006784</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="41"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="60"/>
     </row>
     <row r="10" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="62"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="64"/>
+      <c r="G10" s="70"/>
       <c r="H10" s="7" t="s">
         <v>42</v>
       </c>
@@ -2526,78 +2742,78 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="57"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="4">
         <v>1165006784</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="65"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="25" t="s">
         <v>52</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="69" t="s">
+      <c r="K11" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="69"/>
-      <c r="M11" s="70"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="76"/>
     </row>
     <row r="12" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="63"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
       <c r="J13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="39" t="s">
+      <c r="K13" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="40"/>
-      <c r="M13" s="41"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="60"/>
     </row>
     <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="23" t="s">
@@ -2608,12 +2824,12 @@
       </c>
     </row>
     <row r="16" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="66"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26" s="1" t="s">
@@ -2637,6 +2853,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="F10:G10"/>
@@ -2647,11 +2868,6 @@
     <mergeCell ref="C12:H16"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2659,7 +2875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D6ED93-AE71-40ED-9E2E-AAB7E96B3DB7}">
   <dimension ref="C3:N33"/>
   <sheetViews>
@@ -2676,39 +2892,39 @@
   <sheetData>
     <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="K5" s="74" t="s">
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="60"/>
+      <c r="K5" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="76"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="80"/>
     </row>
     <row r="6" spans="3:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="56" t="s">
+      <c r="E6" s="52"/>
+      <c r="F6" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="58"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="4"/>
@@ -2731,10 +2947,10 @@
       <c r="C8" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="64"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="19" t="s">
         <v>57</v>
       </c>
@@ -2747,20 +2963,20 @@
       <c r="K8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="42" t="s">
+      <c r="L8" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="43"/>
-      <c r="N8" s="44"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="63"/>
     </row>
     <row r="9" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="40"/>
+      <c r="E9" s="59"/>
       <c r="F9" s="21" t="s">
         <v>58</v>
       </c>
@@ -2776,68 +2992,68 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="72"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="71" t="s">
+      <c r="D10" s="82"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83"/>
       <c r="K10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="42" t="s">
+      <c r="L10" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="43"/>
-      <c r="N10" s="44"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="42"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
       <c r="K11" s="2"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="42"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="63"/>
       <c r="K12" s="2"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
       <c r="K13" s="2"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
       <c r="M14" s="23" t="s">
@@ -2848,29 +3064,29 @@
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
     </row>
     <row r="16" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="45"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="66"/>
     </row>
     <row r="23" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="74" t="s">
+      <c r="F24" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="76"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="80"/>
     </row>
     <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
@@ -2894,11 +3110,11 @@
       <c r="F28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="42" t="s">
+      <c r="G28" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="43"/>
-      <c r="I28" s="44"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="63"/>
     </row>
     <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
@@ -2936,6 +3152,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="F24:I24"/>
     <mergeCell ref="G28:I28"/>
     <mergeCell ref="D6:E6"/>
@@ -2944,11 +3165,6 @@
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="C10:E16"/>
     <mergeCell ref="F10:H16"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
update base y ord
</commit_message>
<xml_diff>
--- a/other/DATA_SISGESTION_Nestor.xlsx
+++ b/other/DATA_SISGESTION_Nestor.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SistemaGestionNestorRey\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20F987E-B860-4606-A279-852E5D149B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BB9473-10BA-45E4-8A12-A8EA759B4217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{64D24DBD-44EE-466C-ADE8-9B0DE2C0EE37}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
-    <sheet name="DISEÑO PAGINA" sheetId="6" r:id="rId2"/>
+    <sheet name="ORDENES" sheetId="6" r:id="rId2"/>
     <sheet name="AUTOS" sheetId="3" r:id="rId3"/>
     <sheet name="CLIENTES" sheetId="4" r:id="rId4"/>
     <sheet name="MARCAS Y MODELOS" sheetId="5" r:id="rId5"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="90">
   <si>
     <t>AUTOS</t>
   </si>
@@ -268,7 +268,46 @@
     <t>Cancelado</t>
   </si>
   <si>
-    <t>LISTADO CLIENTES</t>
+    <t>Crear orden</t>
+  </si>
+  <si>
+    <t>AUTO COMPLETADO POR AUTO</t>
+  </si>
+  <si>
+    <t>LISTA DE AUTOS</t>
+  </si>
+  <si>
+    <t>Crear</t>
+  </si>
+  <si>
+    <t>PROBLEMA CON X COSA</t>
+  </si>
+  <si>
+    <t>EXPLICADO BREVEMENTE</t>
+  </si>
+  <si>
+    <t>HONDA FIT</t>
+  </si>
+  <si>
+    <t>Fecha llegada</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Pendiente de pago</t>
   </si>
 </sst>
 </file>
@@ -312,15 +351,15 @@
       <family val="2"/>
     </font>
     <font>
+      <i/>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FF8900B4"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,8 +392,14 @@
         <bgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -631,11 +676,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFA6A200"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFA6A200"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -737,6 +795,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -749,21 +889,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,70 +910,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -857,9 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -869,6 +933,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -878,10 +945,95 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1700,7 +1852,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,7 +1861,9 @@
     <col min="2" max="2" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="4" max="4" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1772,7 +1926,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,7 +1946,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1806,7 +1960,7 @@
         <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1815,6 +1969,9 @@
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="F6" s="95" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1860,159 +2017,519 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9980C8-7DE9-4675-A99D-20A2352C65BC}">
-  <dimension ref="C2:K15"/>
+  <dimension ref="C3:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:H15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35:W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="94"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="41"/>
-    </row>
+    <row r="3" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="58"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="60"/>
-    </row>
-    <row r="5" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="32"/>
-      <c r="D5" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="34"/>
+      <c r="C4" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
+    </row>
+    <row r="5" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
     </row>
     <row r="6" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="32"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="D6" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="89"/>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="43"/>
+    <row r="7" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
       <c r="H7" s="34"/>
     </row>
     <row r="8" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="32"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
+      <c r="C8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="54"/>
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
       <c r="H8" s="34"/>
     </row>
     <row r="9" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="101" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="58"/>
+      <c r="H10" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="111" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="103" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="16">
+        <v>44761</v>
+      </c>
+      <c r="F11" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="76"/>
+      <c r="H11" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="112" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="114"/>
+      <c r="J12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="112"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="114"/>
+      <c r="J13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="112"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="114"/>
+      <c r="J14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="112"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="114"/>
+      <c r="J15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="115"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="117"/>
+      <c r="J16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="94" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
+      <c r="J22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="76"/>
+      <c r="G23" s="77"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="34"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="50"/>
+      <c r="G25" s="51"/>
+    </row>
+    <row r="26" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
+    </row>
+    <row r="27" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="92" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" s="91"/>
+      <c r="G27" s="93"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+    </row>
+    <row r="29" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="32"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="34"/>
+    </row>
+    <row r="30" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="90" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P35" s="107" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q35" s="108"/>
+      <c r="R35" s="108"/>
+      <c r="S35" s="108"/>
+      <c r="T35" s="108"/>
+      <c r="U35" s="108"/>
+      <c r="V35" s="108"/>
+      <c r="W35" s="109"/>
+    </row>
+    <row r="36" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P36" s="99"/>
+      <c r="Q36" s="100"/>
+      <c r="R36" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="S36" s="81"/>
+      <c r="T36" s="81"/>
+      <c r="U36" s="81"/>
+      <c r="V36" s="100"/>
+      <c r="W36" s="104"/>
+    </row>
+    <row r="37" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P37" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q37" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="R37" s="77"/>
+      <c r="S37" s="102" t="s">
+        <v>10</v>
+      </c>
+      <c r="T37" s="75" t="s">
+        <v>82</v>
+      </c>
+      <c r="U37" s="77"/>
+      <c r="V37" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="W37" s="106">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="38" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P38" s="96"/>
+      <c r="Q38" s="98"/>
+      <c r="R38" s="98"/>
+      <c r="S38" s="98"/>
+      <c r="T38" s="98"/>
+      <c r="U38" s="98"/>
+      <c r="V38" s="98"/>
+      <c r="W38" s="97"/>
+    </row>
+    <row r="39" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P39" s="99"/>
+      <c r="Q39" s="100"/>
+      <c r="R39" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="S39" s="81"/>
+      <c r="T39" s="81"/>
+      <c r="U39" s="81"/>
+      <c r="V39" s="100"/>
+      <c r="W39" s="104"/>
+    </row>
+    <row r="40" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P40" s="96"/>
+      <c r="Q40" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="68"/>
-      <c r="E9" s="7" t="s">
+      <c r="R40" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="S40" s="50"/>
+      <c r="T40" s="98"/>
+      <c r="U40" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="V40" s="49">
+        <v>1565006784</v>
+      </c>
+      <c r="W40" s="51"/>
+    </row>
+    <row r="41" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P41" s="96"/>
+      <c r="Q41" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="7" t="s">
+      <c r="R41" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="S41" s="39"/>
+      <c r="T41" s="98"/>
+      <c r="U41" s="102" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="33">
-        <v>1165006784</v>
-      </c>
-      <c r="F10" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="71"/>
-      <c r="H10" s="25" t="s">
+      <c r="V41" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="85"/>
-    </row>
-    <row r="11" spans="3:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="63"/>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="63"/>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="63"/>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
-    </row>
-    <row r="15" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="66"/>
+      <c r="W41" s="77"/>
+    </row>
+    <row r="42" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P42" s="99"/>
+      <c r="Q42" s="100"/>
+      <c r="R42" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="S42" s="81"/>
+      <c r="T42" s="81"/>
+      <c r="U42" s="81"/>
+      <c r="V42" s="100"/>
+      <c r="W42" s="104"/>
+    </row>
+    <row r="43" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P43" s="101" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q43" s="98" t="s">
+        <v>84</v>
+      </c>
+      <c r="R43" s="105"/>
+      <c r="S43" s="102" t="s">
+        <v>10</v>
+      </c>
+      <c r="T43" s="98" t="s">
+        <v>82</v>
+      </c>
+      <c r="U43" s="105"/>
+      <c r="V43" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="W43" s="106">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="44" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P44" s="96"/>
+      <c r="Q44" s="98"/>
+      <c r="R44" s="98"/>
+      <c r="S44" s="98"/>
+      <c r="T44" s="98"/>
+      <c r="U44" s="98"/>
+      <c r="V44" s="98"/>
+      <c r="W44" s="97"/>
+    </row>
+    <row r="45" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P45" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q45" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="R45" s="105"/>
+      <c r="S45" s="101" t="s">
+        <v>10</v>
+      </c>
+      <c r="T45" s="98" t="s">
+        <v>82</v>
+      </c>
+      <c r="U45" s="105"/>
+      <c r="V45" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="W45" s="97"/>
+    </row>
+    <row r="46" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P46" s="96"/>
+      <c r="Q46" s="98"/>
+      <c r="R46" s="98"/>
+      <c r="S46" s="98"/>
+      <c r="T46" s="98"/>
+      <c r="U46" s="98"/>
+      <c r="V46" s="98"/>
+      <c r="W46" s="97"/>
+    </row>
+    <row r="47" spans="16:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P47" s="99"/>
+      <c r="Q47" s="100"/>
+      <c r="R47" s="100"/>
+      <c r="S47" s="100"/>
+      <c r="T47" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="U47" s="64"/>
+      <c r="V47" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="W47" s="89"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C10:D10"/>
+  <mergeCells count="25">
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="V40:W40"/>
+    <mergeCell ref="R41:S41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="P35:W35"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="R36:U36"/>
+    <mergeCell ref="R39:U39"/>
+    <mergeCell ref="R42:U42"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C12:H16"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E29:F29"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="C11:H15"/>
-    <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2020,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E5F623-2172-4AFE-A1E7-9EB4937D4367}">
   <dimension ref="C3:U38"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,44 +2548,44 @@
   <sheetData>
     <row r="3" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="60"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
     </row>
     <row r="6" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="52"/>
       <c r="H6" s="3"/>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="53"/>
-      <c r="P6" s="55" t="s">
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="74"/>
+      <c r="P6" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="57"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="60"/>
+      <c r="S6" s="61"/>
     </row>
     <row r="7" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
@@ -2098,10 +2615,10 @@
       <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -2219,14 +2736,14 @@
       </c>
     </row>
     <row r="12" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="63"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -2237,14 +2754,14 @@
       <c r="S12" s="3"/>
     </row>
     <row r="13" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="63"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="42"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="50" t="s">
+      <c r="K13" s="37" t="s">
         <v>6</v>
       </c>
       <c r="L13" s="52"/>
@@ -2255,28 +2772,28 @@
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
       <c r="M14" s="3"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="63"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="42"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="23" t="s">
@@ -2295,21 +2812,21 @@
       </c>
     </row>
     <row r="16" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="66"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45"/>
     </row>
     <row r="19" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="41"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="9" t="s">
@@ -2320,12 +2837,12 @@
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="29"/>
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="41"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
     </row>
     <row r="22" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="27"/>
@@ -2335,10 +2852,10 @@
       <c r="J22" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="42" t="s">
+      <c r="K22" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="43"/>
+      <c r="L22" s="54"/>
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="4:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2348,10 +2865,10 @@
       <c r="E23" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="38"/>
+      <c r="G23" s="66"/>
       <c r="J23" s="13"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -2382,10 +2899,10 @@
       <c r="E25" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="38"/>
+      <c r="G25" s="66"/>
       <c r="J25" s="18" t="s">
         <v>35</v>
       </c>
@@ -2404,12 +2921,12 @@
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="29"/>
-      <c r="J26" s="44" t="s">
+      <c r="J26" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="46"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="70"/>
     </row>
     <row r="27" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="7" t="s">
@@ -2420,16 +2937,16 @@
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="29"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="46"/>
-      <c r="P27" s="39" t="s">
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="70"/>
+      <c r="P27" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="40"/>
-      <c r="S27" s="41"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="48"/>
       <c r="U27" s="1" t="s">
         <v>45</v>
       </c>
@@ -2439,10 +2956,10 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="29"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="46"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="70"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
@@ -2456,10 +2973,10 @@
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="29"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="49"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="73"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
@@ -2475,16 +2992,16 @@
       <c r="E30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="F30" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="38"/>
+      <c r="G30" s="66"/>
       <c r="J30" s="5"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="35" t="s">
+      <c r="L30" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="M30" s="36"/>
+      <c r="M30" s="64"/>
       <c r="P30" s="2" t="s">
         <v>15</v>
       </c>
@@ -2599,11 +3116,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="P27:S27"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C12:H16"/>
     <mergeCell ref="L30:M30"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="F25:G25"/>
@@ -2618,6 +3130,11 @@
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="D20:G20"/>
+    <mergeCell ref="P27:S27"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C12:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2630,7 +3147,7 @@
   <dimension ref="C3:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H16"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,38 +3157,38 @@
   <sheetData>
     <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="60"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
     </row>
     <row r="6" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="52"/>
       <c r="H6" s="3"/>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="41"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="48"/>
     </row>
     <row r="7" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
@@ -2683,20 +3200,20 @@
       <c r="J7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="72" t="s">
+      <c r="K7" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="73"/>
-      <c r="M7" s="74"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="77"/>
     </row>
     <row r="8" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -2715,24 +3232,24 @@
       <c r="J9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="58">
+      <c r="K9" s="49">
         <v>1165006784</v>
       </c>
-      <c r="L9" s="59"/>
-      <c r="M9" s="60"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="51"/>
     </row>
     <row r="10" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="68"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="69" t="s">
+      <c r="F10" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="70"/>
+      <c r="G10" s="58"/>
       <c r="H10" s="7" t="s">
         <v>42</v>
       </c>
@@ -2742,78 +3259,78 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="4">
         <v>1165006784</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="71"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="25" t="s">
         <v>52</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="75" t="s">
+      <c r="K11" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="75"/>
-      <c r="M11" s="76"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="79"/>
     </row>
     <row r="12" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="63"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="63"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="42"/>
       <c r="J13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="59"/>
-      <c r="M13" s="60"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="51"/>
     </row>
     <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="63"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="42"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="23" t="s">
@@ -2824,12 +3341,12 @@
       </c>
     </row>
     <row r="16" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="66"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26" s="1" t="s">
@@ -2853,11 +3370,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="D8:E8"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="F10:G10"/>
@@ -2868,6 +3380,11 @@
     <mergeCell ref="C12:H16"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2880,7 +3397,7 @@
   <dimension ref="C3:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K5" sqref="K5:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2892,36 +3409,36 @@
   <sheetData>
     <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="60"/>
-      <c r="K5" s="78" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
+      <c r="K5" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="80"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="82"/>
     </row>
     <row r="6" spans="3:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="37" t="s">
         <v>53</v>
       </c>
       <c r="E6" s="52"/>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="37" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="52"/>
@@ -2947,10 +3464,10 @@
       <c r="C8" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="70"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="19" t="s">
         <v>57</v>
       </c>
@@ -2963,20 +3480,20 @@
       <c r="K8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="61" t="s">
+      <c r="L8" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="62"/>
-      <c r="N8" s="63"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="42"/>
     </row>
     <row r="9" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="59"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="21" t="s">
         <v>58</v>
       </c>
@@ -2992,68 +3509,68 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="81" t="s">
+      <c r="D10" s="85"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="86"/>
       <c r="K10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="61" t="s">
+      <c r="L10" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="42"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="63"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="42"/>
       <c r="K11" s="2"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="63"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
       <c r="K12" s="2"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="63"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="42"/>
       <c r="K13" s="2"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
       <c r="M14" s="23" t="s">
@@ -3064,29 +3581,29 @@
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="63"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="42"/>
     </row>
     <row r="16" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="66"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45"/>
     </row>
     <row r="23" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="78" t="s">
+      <c r="F24" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="80"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="82"/>
     </row>
     <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
@@ -3110,11 +3627,11 @@
       <c r="F28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="61" t="s">
+      <c r="G28" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="62"/>
-      <c r="I28" s="63"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="42"/>
     </row>
     <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
@@ -3152,11 +3669,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="F24:I24"/>
     <mergeCell ref="G28:I28"/>
     <mergeCell ref="D6:E6"/>
@@ -3165,6 +3677,11 @@
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="C10:E16"/>
     <mergeCell ref="F10:H16"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualiza menu y agrega finanzas
</commit_message>
<xml_diff>
--- a/other/DATA_SISGESTION_Nestor.xlsx
+++ b/other/DATA_SISGESTION_Nestor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SistemaGestionNestorRey\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61BD03C-499D-4D43-893C-B2F1100934D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBC8E53-28A8-46CA-A144-41788C6E46CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64D24DBD-44EE-466C-ADE8-9B0DE2C0EE37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{64D24DBD-44EE-466C-ADE8-9B0DE2C0EE37}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="CLIENTES" sheetId="4" r:id="rId4"/>
     <sheet name="MARCAS Y MODELOS" sheetId="5" r:id="rId5"/>
     <sheet name="FUNCIONALIDADES" sheetId="7" r:id="rId6"/>
+    <sheet name="FINANZAS" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="137">
   <si>
     <t>AUTOS</t>
   </si>
@@ -420,12 +421,45 @@
   </si>
   <si>
     <t>precio_total</t>
+  </si>
+  <si>
+    <t>Ingresos</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>LISTADO INGRESOS</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Finanzas</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Mano de obra</t>
+  </si>
+  <si>
+    <t>HDC940 - Hona Fit</t>
+  </si>
+  <si>
+    <t>Tomas Berrojalviz</t>
+  </si>
+  <si>
+    <t>Ingresos de Noviembre del 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -836,7 +870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1010,6 +1044,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1214,11 +1281,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2037,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039C5167-16CD-44EC-8879-3C40CCDAB863}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -2232,7 +2305,7 @@
       <c r="G8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I8" s="131"/>
+      <c r="I8" s="66"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
@@ -2258,7 +2331,7 @@
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="132"/>
+      <c r="L13" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2270,8 +2343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9980C8-7DE9-4675-A99D-20A2352C65BC}">
   <dimension ref="C3:W50"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,31 +2357,31 @@
   <sheetData>
     <row r="3" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="63"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="83"/>
     </row>
     <row r="6" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="32"/>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="75"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="34"/>
     </row>
     <row r="7" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2323,10 +2396,10 @@
       <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
       <c r="H8" s="34"/>
@@ -2349,10 +2422,10 @@
       <c r="E10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="68" t="s">
+      <c r="F10" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="69"/>
+      <c r="G10" s="80"/>
       <c r="H10" s="7" t="s">
         <v>46</v>
       </c>
@@ -2367,23 +2440,23 @@
       <c r="E11" s="16">
         <v>44761</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="65"/>
+      <c r="G11" s="76"/>
       <c r="H11" s="34" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="3:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="91"/>
       <c r="J12" s="1" t="s">
         <v>82</v>
       </c>
@@ -2392,12 +2465,12 @@
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="78"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="80"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="91"/>
       <c r="J13" s="1" t="s">
         <v>15</v>
       </c>
@@ -2406,12 +2479,12 @@
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="78"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="80"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="91"/>
       <c r="J14" s="1" t="s">
         <v>16</v>
       </c>
@@ -2420,12 +2493,12 @@
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="78"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="80"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="91"/>
       <c r="J15" s="1" t="s">
         <v>17</v>
       </c>
@@ -2434,12 +2507,12 @@
       </c>
     </row>
     <row r="16" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="81"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="82"/>
-      <c r="H16" s="83"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="94"/>
       <c r="J16" s="1" t="s">
         <v>18</v>
       </c>
@@ -2479,12 +2552,12 @@
       </c>
     </row>
     <row r="22" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="63"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="74"/>
       <c r="J22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2496,11 +2569,11 @@
       <c r="D23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="64" t="s">
+      <c r="E23" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="77"/>
       <c r="J23" s="1"/>
       <c r="O23" s="60"/>
     </row>
@@ -2515,11 +2588,11 @@
       <c r="D25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="71"/>
-      <c r="G25" s="72"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="83"/>
     </row>
     <row r="26" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="32"/>
@@ -2531,24 +2604,24 @@
       <c r="D27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="84" t="s">
+      <c r="E27" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="85"/>
-      <c r="G27" s="86"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="97"/>
     </row>
     <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D28" s="70" t="s">
+      <c r="D28" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="72"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="83"/>
     </row>
     <row r="29" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="32"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
       <c r="G29" s="34"/>
     </row>
     <row r="30" spans="4:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2563,26 +2636,26 @@
     </row>
     <row r="34" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P35" s="91" t="s">
+      <c r="P35" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="Q35" s="92"/>
-      <c r="R35" s="92"/>
-      <c r="S35" s="92"/>
-      <c r="T35" s="92"/>
-      <c r="U35" s="92"/>
-      <c r="V35" s="92"/>
-      <c r="W35" s="93"/>
+      <c r="Q35" s="103"/>
+      <c r="R35" s="103"/>
+      <c r="S35" s="103"/>
+      <c r="T35" s="103"/>
+      <c r="U35" s="103"/>
+      <c r="V35" s="103"/>
+      <c r="W35" s="104"/>
     </row>
     <row r="36" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P36" s="43"/>
       <c r="Q36" s="44"/>
-      <c r="R36" s="89" t="s">
+      <c r="R36" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="S36" s="89"/>
-      <c r="T36" s="89"/>
-      <c r="U36" s="89"/>
+      <c r="S36" s="100"/>
+      <c r="T36" s="100"/>
+      <c r="U36" s="100"/>
       <c r="V36" s="44"/>
       <c r="W36" s="48"/>
     </row>
@@ -2590,17 +2663,17 @@
       <c r="P37" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q37" s="64" t="s">
+      <c r="Q37" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="R37" s="66"/>
+      <c r="R37" s="77"/>
       <c r="S37" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="T37" s="64" t="s">
+      <c r="T37" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="U37" s="66"/>
+      <c r="U37" s="77"/>
       <c r="V37" s="46" t="s">
         <v>12</v>
       </c>
@@ -2621,12 +2694,12 @@
     <row r="39" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P39" s="43"/>
       <c r="Q39" s="44"/>
-      <c r="R39" s="89" t="s">
+      <c r="R39" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="S39" s="89"/>
-      <c r="T39" s="89"/>
-      <c r="U39" s="89"/>
+      <c r="S39" s="100"/>
+      <c r="T39" s="100"/>
+      <c r="U39" s="100"/>
       <c r="V39" s="44"/>
       <c r="W39" s="48"/>
     </row>
@@ -2635,46 +2708,46 @@
       <c r="Q40" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="R40" s="71" t="s">
+      <c r="R40" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="S40" s="71"/>
+      <c r="S40" s="82"/>
       <c r="T40" s="42"/>
       <c r="U40" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="V40" s="70">
+      <c r="V40" s="81">
         <v>1565006784</v>
       </c>
-      <c r="W40" s="72"/>
+      <c r="W40" s="83"/>
     </row>
     <row r="41" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P41" s="40"/>
       <c r="Q41" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="R41" s="90" t="s">
+      <c r="R41" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="S41" s="90"/>
+      <c r="S41" s="101"/>
       <c r="T41" s="42"/>
       <c r="U41" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="V41" s="64" t="s">
+      <c r="V41" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="W41" s="66"/>
+      <c r="W41" s="77"/>
     </row>
     <row r="42" spans="16:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P42" s="43"/>
       <c r="Q42" s="44"/>
-      <c r="R42" s="89" t="s">
+      <c r="R42" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="S42" s="89"/>
-      <c r="T42" s="89"/>
-      <c r="U42" s="89"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="100"/>
+      <c r="U42" s="100"/>
       <c r="V42" s="44"/>
       <c r="W42" s="48"/>
     </row>
@@ -2706,25 +2779,25 @@
     </row>
     <row r="45" spans="16:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P45" s="54"/>
-      <c r="Q45" s="94" t="s">
+      <c r="Q45" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="R45" s="64" t="s">
+      <c r="R45" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="S45" s="65"/>
-      <c r="T45" s="65"/>
-      <c r="U45" s="66"/>
+      <c r="S45" s="76"/>
+      <c r="T45" s="76"/>
+      <c r="U45" s="77"/>
       <c r="V45" s="53"/>
       <c r="W45" s="55"/>
     </row>
     <row r="46" spans="16:23" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P46" s="54"/>
-      <c r="Q46" s="95"/>
-      <c r="R46" s="96"/>
-      <c r="S46" s="67"/>
-      <c r="T46" s="67"/>
-      <c r="U46" s="97"/>
+      <c r="Q46" s="106"/>
+      <c r="R46" s="107"/>
+      <c r="S46" s="78"/>
+      <c r="T46" s="78"/>
+      <c r="U46" s="108"/>
       <c r="V46" s="53"/>
       <c r="W46" s="55"/>
     </row>
@@ -2739,20 +2812,20 @@
       <c r="W47" s="41"/>
     </row>
     <row r="48" spans="16:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P48" s="87" t="s">
+      <c r="P48" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="Q48" s="88"/>
+      <c r="Q48" s="99"/>
       <c r="R48" s="49"/>
-      <c r="S48" s="87" t="s">
+      <c r="S48" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="T48" s="88"/>
+      <c r="T48" s="99"/>
       <c r="U48" s="49"/>
-      <c r="V48" s="87" t="s">
+      <c r="V48" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="W48" s="88"/>
+      <c r="W48" s="99"/>
     </row>
     <row r="49" spans="16:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P49" s="40"/>
@@ -2769,14 +2842,14 @@
       <c r="Q50" s="44"/>
       <c r="R50" s="44"/>
       <c r="S50" s="44"/>
-      <c r="T50" s="87" t="s">
+      <c r="T50" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="U50" s="88"/>
-      <c r="V50" s="73" t="s">
+      <c r="U50" s="99"/>
+      <c r="V50" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="W50" s="75"/>
+      <c r="W50" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -2821,7 +2894,7 @@
   <dimension ref="C3:U38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:K7"/>
+      <selection activeCell="J21" sqref="J21:M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,44 +2904,44 @@
   <sheetData>
     <row r="3" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="63"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="83"/>
     </row>
     <row r="6" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="116" t="s">
+      <c r="D6" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="118"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="129"/>
       <c r="H6" s="3"/>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="119"/>
-      <c r="P6" s="98" t="s">
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="130"/>
+      <c r="P6" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="99"/>
-      <c r="S6" s="100"/>
+      <c r="Q6" s="110"/>
+      <c r="R6" s="110"/>
+      <c r="S6" s="111"/>
     </row>
     <row r="7" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
@@ -2898,10 +2971,10 @@
       <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="109" t="s">
+      <c r="D8" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -3019,14 +3092,14 @@
       </c>
     </row>
     <row r="12" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="101" t="s">
+      <c r="C12" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="103"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="114"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -3037,17 +3110,17 @@
       <c r="S12" s="3"/>
     </row>
     <row r="13" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="101"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="103"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="114"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="116" t="s">
+      <c r="K13" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="118"/>
+      <c r="L13" s="129"/>
       <c r="M13" s="3"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="4"/>
@@ -3055,28 +3128,28 @@
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="103"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="114"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
       <c r="M14" s="3"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="67"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="103"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="114"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="23" t="s">
@@ -3095,21 +3168,21 @@
       </c>
     </row>
     <row r="16" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="104"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="106"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="117"/>
     </row>
     <row r="19" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="63"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="74"/>
     </row>
     <row r="21" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="9" t="s">
@@ -3120,12 +3193,12 @@
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="29"/>
-      <c r="J21" s="61" t="s">
+      <c r="J21" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="K21" s="62"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="63"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="74"/>
     </row>
     <row r="22" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="27"/>
@@ -3135,10 +3208,10 @@
       <c r="J22" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="109" t="s">
+      <c r="K22" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="77"/>
+      <c r="L22" s="88"/>
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="4:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3148,10 +3221,10 @@
       <c r="E23" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="107" t="s">
+      <c r="F23" s="118" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="108"/>
+      <c r="G23" s="119"/>
       <c r="J23" s="13"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -3182,10 +3255,10 @@
       <c r="E25" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="107" t="s">
+      <c r="F25" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="108"/>
+      <c r="G25" s="119"/>
       <c r="J25" s="18" t="s">
         <v>35</v>
       </c>
@@ -3204,12 +3277,12 @@
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="29"/>
-      <c r="J26" s="110" t="s">
+      <c r="J26" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="K26" s="111"/>
-      <c r="L26" s="111"/>
-      <c r="M26" s="112"/>
+      <c r="K26" s="122"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="123"/>
     </row>
     <row r="27" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="7" t="s">
@@ -3220,16 +3293,16 @@
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="29"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111"/>
-      <c r="M27" s="112"/>
-      <c r="P27" s="61" t="s">
+      <c r="J27" s="121"/>
+      <c r="K27" s="122"/>
+      <c r="L27" s="122"/>
+      <c r="M27" s="123"/>
+      <c r="P27" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="Q27" s="62"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="63"/>
+      <c r="Q27" s="73"/>
+      <c r="R27" s="73"/>
+      <c r="S27" s="74"/>
       <c r="U27" s="1" t="s">
         <v>45</v>
       </c>
@@ -3239,10 +3312,10 @@
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="29"/>
-      <c r="J28" s="110"/>
-      <c r="K28" s="111"/>
-      <c r="L28" s="111"/>
-      <c r="M28" s="112"/>
+      <c r="J28" s="121"/>
+      <c r="K28" s="122"/>
+      <c r="L28" s="122"/>
+      <c r="M28" s="123"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
@@ -3256,10 +3329,10 @@
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
       <c r="G29" s="29"/>
-      <c r="J29" s="113"/>
-      <c r="K29" s="114"/>
-      <c r="L29" s="114"/>
-      <c r="M29" s="115"/>
+      <c r="J29" s="124"/>
+      <c r="K29" s="125"/>
+      <c r="L29" s="125"/>
+      <c r="M29" s="126"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
@@ -3275,16 +3348,16 @@
       <c r="E30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="107" t="s">
+      <c r="F30" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="G30" s="108"/>
+      <c r="G30" s="119"/>
       <c r="J30" s="5"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="87" t="s">
+      <c r="L30" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="M30" s="88"/>
+      <c r="M30" s="99"/>
       <c r="P30" s="2" t="s">
         <v>15</v>
       </c>
@@ -3440,38 +3513,38 @@
   <sheetData>
     <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="63"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="83"/>
     </row>
     <row r="6" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="116" t="s">
+      <c r="D6" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="118"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="129"/>
       <c r="H6" s="3"/>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="63"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="74"/>
     </row>
     <row r="7" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
@@ -3483,20 +3556,20 @@
       <c r="J7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="64" t="s">
+      <c r="K7" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="65"/>
-      <c r="M7" s="66"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="77"/>
     </row>
     <row r="8" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
@@ -3515,24 +3588,24 @@
       <c r="J9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="70">
+      <c r="K9" s="81">
         <v>1165006784</v>
       </c>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="83"/>
     </row>
     <row r="10" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="120" t="s">
+      <c r="C10" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="121"/>
+      <c r="D10" s="132"/>
       <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="68" t="s">
+      <c r="F10" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="69"/>
+      <c r="G10" s="80"/>
       <c r="H10" s="7" t="s">
         <v>42</v>
       </c>
@@ -3542,78 +3615,78 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="117"/>
+      <c r="D11" s="128"/>
       <c r="E11" s="4">
         <v>1165006784</v>
       </c>
-      <c r="F11" s="90" t="s">
+      <c r="F11" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="90"/>
+      <c r="G11" s="101"/>
       <c r="H11" s="25" t="s">
         <v>52</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="122" t="s">
+      <c r="K11" s="133" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="122"/>
-      <c r="M11" s="123"/>
+      <c r="L11" s="133"/>
+      <c r="M11" s="134"/>
     </row>
     <row r="12" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="101" t="s">
+      <c r="C12" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="103"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="114"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="101"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="103"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="114"/>
       <c r="J13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="70" t="s">
+      <c r="K13" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="71"/>
-      <c r="M13" s="72"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="83"/>
     </row>
     <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="103"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="114"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="3:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="103"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="114"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="23" t="s">
@@ -3624,12 +3697,12 @@
       </c>
     </row>
     <row r="16" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="104"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="106"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="117"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26" s="1" t="s">
@@ -3692,39 +3765,39 @@
   <sheetData>
     <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="63"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74"/>
     </row>
     <row r="5" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
-      <c r="K5" s="124" t="s">
+      <c r="C5" s="81"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="83"/>
+      <c r="K5" s="135" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="125"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="136"/>
     </row>
     <row r="6" spans="3:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
-      <c r="D6" s="116" t="s">
+      <c r="D6" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="118"/>
-      <c r="F6" s="116" t="s">
+      <c r="E6" s="129"/>
+      <c r="F6" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="118"/>
+      <c r="G6" s="129"/>
       <c r="H6" s="3"/>
       <c r="K6" s="2"/>
       <c r="L6" s="4"/>
@@ -3747,10 +3820,10 @@
       <c r="C8" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="126" t="s">
+      <c r="D8" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="69"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="19" t="s">
         <v>57</v>
       </c>
@@ -3763,20 +3836,20 @@
       <c r="K8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="101" t="s">
+      <c r="L8" s="112" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="114"/>
     </row>
     <row r="9" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="71"/>
+      <c r="E9" s="82"/>
       <c r="F9" s="21" t="s">
         <v>58</v>
       </c>
@@ -3792,68 +3865,68 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="127" t="s">
+      <c r="C10" s="138" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="128"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="127" t="s">
+      <c r="D10" s="139"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="138" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="128"/>
-      <c r="H10" s="129"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="140"/>
       <c r="K10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="101" t="s">
+      <c r="L10" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="102"/>
-      <c r="N10" s="103"/>
+      <c r="M10" s="113"/>
+      <c r="N10" s="114"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="101"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="103"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="114"/>
       <c r="K11" s="2"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="101"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="103"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="114"/>
       <c r="K12" s="2"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="101"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="103"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="114"/>
       <c r="K13" s="2"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="103"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="114"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="114"/>
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
       <c r="M14" s="23" t="s">
@@ -3864,29 +3937,29 @@
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="103"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="114"/>
     </row>
     <row r="16" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="104"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="106"/>
-      <c r="F16" s="104"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="106"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="115"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="117"/>
     </row>
     <row r="23" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="124" t="s">
+      <c r="F24" s="135" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="89"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="125"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="136"/>
     </row>
     <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
@@ -3910,11 +3983,11 @@
       <c r="F28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="101" t="s">
+      <c r="G28" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="102"/>
-      <c r="I28" s="103"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="114"/>
     </row>
     <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
@@ -3976,7 +4049,7 @@
   <dimension ref="D3:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,11 +4066,11 @@
   <sheetData>
     <row r="3" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="130" t="s">
+      <c r="D4" s="141" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
     </row>
     <row r="5" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="58" t="s">
@@ -4130,4 +4203,261 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E856FE-06D4-422B-A3B6-10CED06CE50F}">
+  <dimension ref="B2:P29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20:P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="11.42578125" style="39"/>
+    <col min="13" max="13" width="6.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="16.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="74"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="81"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="83"/>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="63"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="88"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="63"/>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="61"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="63"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="80"/>
+      <c r="D8" s="79" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="80"/>
+      <c r="F8" s="137" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="80"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="142">
+        <v>2022</v>
+      </c>
+      <c r="C9" s="143"/>
+      <c r="D9" s="144" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="144"/>
+      <c r="F9" s="145">
+        <v>10000</v>
+      </c>
+      <c r="G9" s="77"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="89" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="91"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="89"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="91"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="89"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="91"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="89"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="91"/>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="92"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="94"/>
+    </row>
+    <row r="19" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="74"/>
+    </row>
+    <row r="21" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="120" t="s">
+        <v>32</v>
+      </c>
+      <c r="N21" s="88"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="63"/>
+    </row>
+    <row r="22" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="69"/>
+      <c r="M22" s="70"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="63"/>
+    </row>
+    <row r="23" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="M23" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="N23" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="O23" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23" s="45" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="12:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="71">
+        <v>44882</v>
+      </c>
+      <c r="M24" s="23">
+        <v>3</v>
+      </c>
+      <c r="N24" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="O24" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="P24" s="68">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="25" spans="12:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="121" t="s">
+        <v>49</v>
+      </c>
+      <c r="M25" s="122"/>
+      <c r="N25" s="122"/>
+      <c r="O25" s="122"/>
+      <c r="P25" s="123"/>
+    </row>
+    <row r="26" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L26" s="121"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
+      <c r="O26" s="122"/>
+      <c r="P26" s="123"/>
+    </row>
+    <row r="27" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L27" s="121"/>
+      <c r="M27" s="122"/>
+      <c r="N27" s="122"/>
+      <c r="O27" s="122"/>
+      <c r="P27" s="123"/>
+    </row>
+    <row r="28" spans="12:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="121"/>
+      <c r="M28" s="122"/>
+      <c r="N28" s="122"/>
+      <c r="O28" s="122"/>
+      <c r="P28" s="123"/>
+    </row>
+    <row r="29" spans="12:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L29" s="65"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="98" t="s">
+        <v>61</v>
+      </c>
+      <c r="P29" s="99"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="L20:P20"/>
+    <mergeCell ref="L25:P28"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="B10:G14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>